<commit_message>
Translation updated but need to be tested again
</commit_message>
<xml_diff>
--- a/out/RMRP_2021_AI_consolidated.xlsx
+++ b/out/RMRP_2021_AI_consolidated.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -655,16 +655,16 @@
         </is>
       </c>
       <c r="E4">
-        <v>1229</v>
+        <v>1267</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="H4">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -679,16 +679,16 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O4">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="P4">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -1065,16 +1065,16 @@
         </is>
       </c>
       <c r="E9">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="H9">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1089,16 +1089,16 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="P9">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1475,40 +1475,40 @@
         </is>
       </c>
       <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
         <v>1</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
       <c r="O14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1557,16 +1557,16 @@
         </is>
       </c>
       <c r="E15">
-        <v>1356</v>
+        <v>1475</v>
       </c>
       <c r="F15">
         <v>35</v>
       </c>
       <c r="G15">
-        <v>172</v>
+        <v>125</v>
       </c>
       <c r="H15">
-        <v>172</v>
+        <v>125</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1581,16 +1581,16 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N15">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="O15">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="P15">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -1599,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -1612,1154 +1612,6 @@
         </is>
       </c>
       <c r="V15" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Education</t>
-        </is>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Food Security</t>
-        </is>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>9</v>
-      </c>
-      <c r="H17">
-        <v>9</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>3</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="O17">
-        <v>2</v>
-      </c>
-      <c r="P17">
-        <v>3</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>9</v>
-      </c>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Health</t>
-        </is>
-      </c>
-      <c r="E18">
-        <v>38</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>83</v>
-      </c>
-      <c r="H18">
-        <v>83</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>7</v>
-      </c>
-      <c r="N18">
-        <v>5</v>
-      </c>
-      <c r="O18">
-        <v>56</v>
-      </c>
-      <c r="P18">
-        <v>15</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V18" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Humanitarian Transportation</t>
-        </is>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V19" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Integration</t>
-        </is>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>36</v>
-      </c>
-      <c r="H20">
-        <v>36</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>26</v>
-      </c>
-      <c r="P20">
-        <v>9</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V20" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Multipurpose Cash Assistance (MPC)</t>
-        </is>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>26</v>
-      </c>
-      <c r="H21">
-        <v>26</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>5</v>
-      </c>
-      <c r="N21">
-        <v>3</v>
-      </c>
-      <c r="O21">
-        <v>10</v>
-      </c>
-      <c r="P21">
-        <v>8</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>26</v>
-      </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V21" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Nutrition</t>
-        </is>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V22" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Protection (General)</t>
-        </is>
-      </c>
-      <c r="E23">
-        <v>72</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>124</v>
-      </c>
-      <c r="H23">
-        <v>124</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>78</v>
-      </c>
-      <c r="P23">
-        <v>45</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Protection (GBV)</t>
-        </is>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>2</v>
-      </c>
-      <c r="H24">
-        <v>2</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>2</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Protection (Human Trafficking and Smuggling)</t>
-        </is>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V25" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Protection (Child Protection)</t>
-        </is>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V26" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Shelter</t>
-        </is>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>1</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="T27" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V27" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>WASH</t>
-        </is>
-      </c>
-      <c r="E28">
-        <v>9</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>10</v>
-      </c>
-      <c r="H28">
-        <v>10</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>4</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-      <c r="O28">
-        <v>2</v>
-      </c>
-      <c r="P28">
-        <v>3</v>
-      </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V28" t="inlineStr">
-        <is>
-          <t>ok</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Central America and Mexico</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Costa Rica</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>2022-02</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Intersector</t>
-        </is>
-      </c>
-      <c r="E29">
-        <v>119</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>291</v>
-      </c>
-      <c r="H29">
-        <v>291</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>21</v>
-      </c>
-      <c r="N29">
-        <v>10</v>
-      </c>
-      <c r="O29">
-        <v>176</v>
-      </c>
-      <c r="P29">
-        <v>84</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
-      <c r="S29">
-        <v>35</v>
-      </c>
-      <c r="T29" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="V29" t="inlineStr">
         <is>
           <t>ok</t>
         </is>

</xml_diff>

<commit_message>
App pending deployment Translation and DQC in Spanish working but needed to be integrated to app
</commit_message>
<xml_diff>
--- a/out/RMRP_2021_AI_consolidated.xlsx
+++ b/out/RMRP_2021_AI_consolidated.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1692,6 +1692,1224 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Education</t>
+        </is>
+      </c>
+      <c r="F16">
+        <v>88</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>88</v>
+      </c>
+      <c r="I16">
+        <v>88</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>68</v>
+      </c>
+      <c r="Q16">
+        <v>18</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Food Security</t>
+        </is>
+      </c>
+      <c r="F17">
+        <v>47</v>
+      </c>
+      <c r="G17">
+        <v>41</v>
+      </c>
+      <c r="H17">
+        <v>56</v>
+      </c>
+      <c r="I17">
+        <v>56</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>8</v>
+      </c>
+      <c r="O17">
+        <v>9</v>
+      </c>
+      <c r="P17">
+        <v>20</v>
+      </c>
+      <c r="Q17">
+        <v>19</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>50</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Health</t>
+        </is>
+      </c>
+      <c r="F18">
+        <v>1264</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>183</v>
+      </c>
+      <c r="I18">
+        <v>183</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>8</v>
+      </c>
+      <c r="O18">
+        <v>5</v>
+      </c>
+      <c r="P18">
+        <v>117</v>
+      </c>
+      <c r="Q18">
+        <v>53</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Humanitarian Transportation</t>
+        </is>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Integration</t>
+        </is>
+      </c>
+      <c r="F20">
+        <v>79</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>115</v>
+      </c>
+      <c r="I20">
+        <v>115</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>83</v>
+      </c>
+      <c r="Q20">
+        <v>29</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Multipurpose Cash Assistance (MPC)</t>
+        </is>
+      </c>
+      <c r="F21">
+        <v>83</v>
+      </c>
+      <c r="G21">
+        <v>82</v>
+      </c>
+      <c r="H21">
+        <v>84</v>
+      </c>
+      <c r="I21">
+        <v>84</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>18</v>
+      </c>
+      <c r="O21">
+        <v>12</v>
+      </c>
+      <c r="P21">
+        <v>33</v>
+      </c>
+      <c r="Q21">
+        <v>21</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>83</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Nutrition</t>
+        </is>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Protection (General)</t>
+        </is>
+      </c>
+      <c r="F23">
+        <v>172</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>296</v>
+      </c>
+      <c r="I23">
+        <v>296</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>7</v>
+      </c>
+      <c r="O23">
+        <v>5</v>
+      </c>
+      <c r="P23">
+        <v>175</v>
+      </c>
+      <c r="Q23">
+        <v>108</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Protection (GBV)</t>
+        </is>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>3</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Protection (Human Trafficking and Smuggling)</t>
+        </is>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Protection (Child Protection)</t>
+        </is>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Shelter</t>
+        </is>
+      </c>
+      <c r="F27">
+        <v>59</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>60</v>
+      </c>
+      <c r="I27">
+        <v>60</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>8</v>
+      </c>
+      <c r="O27">
+        <v>8</v>
+      </c>
+      <c r="P27">
+        <v>15</v>
+      </c>
+      <c r="Q27">
+        <v>29</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>WASH</t>
+        </is>
+      </c>
+      <c r="F28">
+        <v>42</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>52</v>
+      </c>
+      <c r="I28">
+        <v>52</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>9</v>
+      </c>
+      <c r="O28">
+        <v>8</v>
+      </c>
+      <c r="P28">
+        <v>18</v>
+      </c>
+      <c r="Q28">
+        <v>17</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Central America and Mexico</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Country level</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2022-02</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Intersector</t>
+        </is>
+      </c>
+      <c r="F29">
+        <v>1835</v>
+      </c>
+      <c r="G29">
+        <v>123</v>
+      </c>
+      <c r="H29">
+        <v>937</v>
+      </c>
+      <c r="I29">
+        <v>937</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>63</v>
+      </c>
+      <c r="O29">
+        <v>47</v>
+      </c>
+      <c r="P29">
+        <v>532</v>
+      </c>
+      <c r="Q29">
+        <v>294</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>133</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>